<commit_message>
CONFIRMED  Problem № 5.cs
</commit_message>
<xml_diff>
--- a/Systems conquered the name of the emperor.xlsx
+++ b/Systems conquered the name of the emperor.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
   <si>
     <t>a</t>
   </si>
@@ -426,13 +426,13 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="2" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -469,7 +469,9 @@
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">

</xml_diff>